<commit_message>
force computation from reluctance looks promissing
</commit_message>
<xml_diff>
--- a/design_params_ref.xlsx
+++ b/design_params_ref.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kutla\Documents\Inventor\Micro_High_Speed_Valve\ref\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kutlayhanli/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9344733-C52C-45DF-8E64-7A6DFAC39A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03682904-F73C-5448-B0FE-BCCFD3C1DB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5625" yWindow="2505" windowWidth="21600" windowHeight="12735" xr2:uid="{1FBF37E3-FA93-4DBE-8BE5-46D2802649B7}"/>
+    <workbookView xWindow="5620" yWindow="2500" windowWidth="21600" windowHeight="12740" xr2:uid="{1FBF37E3-FA93-4DBE-8BE5-46D2802649B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -400,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -427,6 +427,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -743,20 +747,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7326A7-BB3C-4FF1-81A0-340B3664836D}">
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -767,7 +771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -778,7 +782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -789,7 +793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -800,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -811,7 +815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>68</v>
       </c>
@@ -822,7 +826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>69</v>
       </c>
@@ -833,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -844,7 +848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -855,7 +859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -866,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -877,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>67</v>
       </c>
@@ -888,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -899,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -910,7 +914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -921,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>87</v>
       </c>
@@ -932,7 +936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>89</v>
       </c>
@@ -943,7 +947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
@@ -954,7 +958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -965,7 +969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -976,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
@@ -987,7 +991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
@@ -998,7 +1002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
@@ -1009,7 +1013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>17</v>
       </c>
@@ -1020,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
@@ -1031,7 +1035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
@@ -1042,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
@@ -1053,7 +1057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>21</v>
       </c>
@@ -1064,7 +1068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>22</v>
       </c>
@@ -1075,7 +1079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
@@ -1086,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>24</v>
       </c>
@@ -1097,7 +1101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>27</v>
       </c>
@@ -1108,7 +1112,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>26</v>
       </c>
@@ -1119,7 +1123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>35</v>
       </c>
@@ -1130,7 +1134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>34</v>
       </c>
@@ -1141,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>33</v>
       </c>
@@ -1152,7 +1156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
@@ -1163,7 +1167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
@@ -1174,7 +1178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
@@ -1185,7 +1189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
@@ -1196,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>90</v>
       </c>
@@ -1205,7 +1209,7 @@
       </c>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>40</v>
       </c>
@@ -1216,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>38</v>
       </c>
@@ -1227,7 +1231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>39</v>
       </c>
@@ -1238,7 +1242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>70</v>
       </c>
@@ -1249,7 +1253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>71</v>
       </c>
@@ -1260,7 +1264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>41</v>
       </c>
@@ -1271,7 +1275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>43</v>
       </c>
@@ -1281,8 +1285,14 @@
       <c r="C48" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+    </row>
+    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>42</v>
       </c>
@@ -1292,8 +1302,14 @@
       <c r="C49" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+    </row>
+    <row r="50" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>44</v>
       </c>
@@ -1303,8 +1319,14 @@
       <c r="C50" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+    </row>
+    <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>46</v>
       </c>
@@ -1314,12 +1336,14 @@
       <c r="C51" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G51" s="1"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F51" s="10"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="10"/>
+    </row>
+    <row r="52" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>47</v>
       </c>
@@ -1329,8 +1353,14 @@
       <c r="C52" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+    </row>
+    <row r="53" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>48</v>
       </c>
@@ -1340,8 +1370,14 @@
       <c r="C53" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+    </row>
+    <row r="54" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>49</v>
       </c>
@@ -1352,7 +1388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>50</v>
       </c>
@@ -1363,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>72</v>
       </c>
@@ -1374,7 +1410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>73</v>
       </c>
@@ -1385,7 +1421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>77</v>
       </c>
@@ -1396,7 +1432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>52</v>
       </c>
@@ -1407,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>53</v>
       </c>
@@ -1418,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>54</v>
       </c>
@@ -1429,7 +1465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
         <v>56</v>
       </c>
@@ -1440,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
         <v>58</v>
       </c>
@@ -1451,7 +1487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
         <v>63</v>
       </c>
@@ -1462,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
         <v>64</v>
       </c>
@@ -1473,7 +1509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
         <v>61</v>
       </c>
@@ -1484,7 +1520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
         <v>65</v>
       </c>
@@ -1495,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>74</v>
       </c>
@@ -1506,7 +1542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>76</v>
       </c>
@@ -1517,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>78</v>
       </c>
@@ -1528,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>79</v>
       </c>
@@ -1539,7 +1575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>80</v>
       </c>
@@ -1550,7 +1586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>81</v>
       </c>
@@ -1561,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>82</v>
       </c>
@@ -1572,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>84</v>
       </c>
@@ -1583,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
Adjusted valve geometry to maximize force. Looks promising
</commit_message>
<xml_diff>
--- a/design_params_ref.xlsx
+++ b/design_params_ref.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kutlayhanli/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03682904-F73C-5448-B0FE-BCCFD3C1DB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE9E39C-04F6-A747-8B3A-09B9B6FEC123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="2500" windowWidth="21600" windowHeight="12740" xr2:uid="{1FBF37E3-FA93-4DBE-8BE5-46D2802649B7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1FBF37E3-FA93-4DBE-8BE5-46D2802649B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="93">
   <si>
     <t>valve_seat_outlet_orifice_d</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>valve_spool_h * 0.8</t>
+  </si>
+  <si>
+    <t>coil_former_dout + 2</t>
   </si>
 </sst>
 </file>
@@ -749,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7326A7-BB3C-4FF1-81A0-340B3664836D}">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1150,7 +1153,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="5">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>1</v>
@@ -1347,8 +1350,8 @@
       <c r="A52" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="7">
-        <v>12</v>
+      <c r="B52" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
increased orifice diameter and fixed bug in winding count
</commit_message>
<xml_diff>
--- a/design_params_ref.xlsx
+++ b/design_params_ref.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kutlayhanli/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA905D2-0D5A-6944-99F3-7D91D1E75469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD79CCC6-83E7-6A44-8FBD-2986B8D5E0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1FBF37E3-FA93-4DBE-8BE5-46D2802649B7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="116">
   <si>
     <t>valve_seat_outlet_orifice_d</t>
   </si>
@@ -313,9 +313,6 @@
     <t>shell_dout + 4</t>
   </si>
   <si>
-    <t>valve_seat_outlet_d - 3</t>
-  </si>
-  <si>
     <t>valve_seat_din + 3</t>
   </si>
   <si>
@@ -383,6 +380,9 @@
   </si>
   <si>
     <t>valve_seat_outlet_face_oring_dout - 2 * face_oring_groove_width</t>
+  </si>
+  <si>
+    <t>coil_dout + 3</t>
   </si>
 </sst>
 </file>
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7326A7-BB3C-4FF1-81A0-340B3664836D}">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -856,7 +856,7 @@
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="1">
         <v>1.78</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="1">
         <v>1.34</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" s="1">
         <v>2.15</v>
@@ -889,7 +889,7 @@
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="1">
         <v>12.81</v>
@@ -900,7 +900,7 @@
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" s="1">
         <v>0.2</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" s="1">
         <v>1.29</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9" s="1">
         <v>2.35</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" s="1">
         <v>20.73</v>
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>1</v>
@@ -991,7 +991,7 @@
         <v>66</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>1</v>
@@ -1002,7 +1002,7 @@
         <v>65</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>1</v>
@@ -1013,7 +1013,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>1</v>
@@ -1046,7 +1046,7 @@
         <v>64</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>1</v>
@@ -1057,7 +1057,7 @@
         <v>63</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>1</v>
@@ -1068,7 +1068,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>1</v>
@@ -1076,10 +1076,10 @@
     </row>
     <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>1</v>
@@ -1087,10 +1087,10 @@
     </row>
     <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>1</v>
@@ -1101,7 +1101,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>1</v>
@@ -1167,7 +1167,7 @@
         <v>13</v>
       </c>
       <c r="B31" s="3">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>1</v>
@@ -1321,7 +1321,7 @@
         <v>33</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>1</v>
@@ -1331,8 +1331,8 @@
       <c r="A46" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>92</v>
+      <c r="B46" s="5">
+        <v>30</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>1</v>
@@ -1376,7 +1376,7 @@
         <v>35</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>1</v>
@@ -1395,10 +1395,10 @@
     </row>
     <row r="52" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>1</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="53" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>1</v>
@@ -1417,10 +1417,10 @@
     </row>
     <row r="54" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>1</v>
@@ -1565,7 +1565,7 @@
         <v>45</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>3</v>
+        <v>115</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>1</v>
@@ -1665,7 +1665,7 @@
         <v>51</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>1</v>
@@ -1687,7 +1687,7 @@
         <v>54</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>1</v>
@@ -1731,7 +1731,7 @@
         <v>59</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C79" s="9" t="s">
         <v>1</v>
@@ -1775,7 +1775,7 @@
         <v>75</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>1</v>
@@ -1786,7 +1786,7 @@
         <v>74</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>1</v>
@@ -1797,7 +1797,7 @@
         <v>76</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>1</v>
@@ -1808,7 +1808,7 @@
         <v>77</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Decided on cone squeeze
</commit_message>
<xml_diff>
--- a/design_params_ref.xlsx
+++ b/design_params_ref.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kutlayhanli/thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kutla\Documents\GitHub\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD79CCC6-83E7-6A44-8FBD-2986B8D5E0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7F3DA4-0B20-4195-959B-B8EA553A39F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1FBF37E3-FA93-4DBE-8BE5-46D2802649B7}"/>
+    <workbookView xWindow="5625" yWindow="2505" windowWidth="21600" windowHeight="12735" xr2:uid="{1FBF37E3-FA93-4DBE-8BE5-46D2802649B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="117">
   <si>
     <t>valve_seat_outlet_orifice_d</t>
   </si>
@@ -383,6 +383,9 @@
   </si>
   <si>
     <t>coil_dout + 3</t>
+  </si>
+  <si>
+    <t>valve_cone_cone_d / 2</t>
   </si>
 </sst>
 </file>
@@ -821,18 +824,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7326A7-BB3C-4FF1-81A0-340B3664836D}">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
@@ -843,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
@@ -854,7 +857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
@@ -865,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>105</v>
       </c>
@@ -876,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>106</v>
       </c>
@@ -887,7 +890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>104</v>
       </c>
@@ -898,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>97</v>
       </c>
@@ -909,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>101</v>
       </c>
@@ -920,7 +923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>102</v>
       </c>
@@ -931,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>103</v>
       </c>
@@ -942,7 +945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -953,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -964,7 +967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -975,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -986,7 +989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>66</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -1041,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>64</v>
       </c>
@@ -1052,7 +1055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -1063,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -1074,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>107</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>108</v>
       </c>
@@ -1096,7 +1099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -1107,7 +1110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>83</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>84</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
@@ -1140,29 +1143,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="3">
-        <v>3</v>
+      <c r="B29" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B30" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>13</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>14</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>15</v>
       </c>
@@ -1195,7 +1198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>16</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>17</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>18</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>19</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>20</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>21</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>22</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>23</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>26</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>25</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>34</v>
       </c>
@@ -1316,7 +1319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>33</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>32</v>
       </c>
@@ -1338,7 +1341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>29</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>30</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>31</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>35</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>98</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>99</v>
       </c>
@@ -1415,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>100</v>
       </c>
@@ -1426,7 +1429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>38</v>
       </c>
@@ -1437,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>36</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>37</v>
       </c>
@@ -1459,7 +1462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>67</v>
       </c>
@@ -1470,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>68</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>39</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>41</v>
       </c>
@@ -1509,7 +1512,7 @@
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
     </row>
-    <row r="62" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>40</v>
       </c>
@@ -1526,7 +1529,7 @@
       <c r="J62" s="10"/>
       <c r="K62" s="10"/>
     </row>
-    <row r="63" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>42</v>
       </c>
@@ -1543,7 +1546,7 @@
       <c r="J63" s="10"/>
       <c r="K63" s="10"/>
     </row>
-    <row r="64" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>44</v>
       </c>
@@ -1560,7 +1563,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="10"/>
     </row>
-    <row r="65" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>45</v>
       </c>
@@ -1577,7 +1580,7 @@
       <c r="J65" s="10"/>
       <c r="K65" s="10"/>
     </row>
-    <row r="66" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>46</v>
       </c>
@@ -1594,7 +1597,7 @@
       <c r="J66" s="10"/>
       <c r="K66" s="10"/>
     </row>
-    <row r="67" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>47</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>48</v>
       </c>
@@ -1616,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>69</v>
       </c>
@@ -1627,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>70</v>
       </c>
@@ -1638,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>73</v>
       </c>
@@ -1649,7 +1652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>50</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>51</v>
       </c>
@@ -1671,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>52</v>
       </c>
@@ -1682,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>54</v>
       </c>
@@ -1693,7 +1696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>56</v>
       </c>
@@ -1704,7 +1707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>60</v>
       </c>
@@ -1715,7 +1718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>61</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>59</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>62</v>
       </c>
@@ -1748,7 +1751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>71</v>
       </c>
@@ -1759,7 +1762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>72</v>
       </c>
@@ -1770,7 +1773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>75</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>74</v>
       </c>
@@ -1792,7 +1795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>76</v>
       </c>
@@ -1803,7 +1806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>77</v>
       </c>
@@ -1814,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>78</v>
       </c>
@@ -1825,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>80</v>
       </c>
@@ -1836,7 +1839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
Direct acting high flow rate design
</commit_message>
<xml_diff>
--- a/design_params_ref.xlsx
+++ b/design_params_ref.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kutla\Documents\GitHub\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7F3DA4-0B20-4195-959B-B8EA553A39F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1ACBF4F-6515-4D08-8CC5-0B39BCAC0263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5625" yWindow="2505" windowWidth="21600" windowHeight="12735" xr2:uid="{1FBF37E3-FA93-4DBE-8BE5-46D2802649B7}"/>
   </bookViews>
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7326A7-BB3C-4FF1-81A0-340B3664836D}">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,7 +840,7 @@
         <v>55</v>
       </c>
       <c r="B1" s="1">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -950,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="2">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>1</v>
@@ -1313,7 +1313,7 @@
         <v>34</v>
       </c>
       <c r="B44" s="5">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>1</v>
@@ -1335,7 +1335,7 @@
         <v>32</v>
       </c>
       <c r="B46" s="5">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>1</v>
@@ -1517,7 +1517,7 @@
         <v>40</v>
       </c>
       <c r="B62" s="7">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>1</v>

</xml_diff>